<commit_message>
Halfway through changing method used in cut to software function
</commit_message>
<xml_diff>
--- a/outputs/Title.xlsx
+++ b/outputs/Title.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="456">
   <si>
     <t>Case Study Id</t>
   </si>
@@ -41,6 +41,51 @@
   </si>
   <si>
     <t xml:space="preserve">Sources to corroborate the impact </t>
+  </si>
+  <si>
+    <t>ahrc</t>
+  </si>
+  <si>
+    <t>bbsrc</t>
+  </si>
+  <si>
+    <t>british_academy</t>
+  </si>
+  <si>
+    <t>cclrc</t>
+  </si>
+  <si>
+    <t>epsrc</t>
+  </si>
+  <si>
+    <t>esrc</t>
+  </si>
+  <si>
+    <t>mrc</t>
+  </si>
+  <si>
+    <t>nerc</t>
+  </si>
+  <si>
+    <t>pparc</t>
+  </si>
+  <si>
+    <t>rcuk</t>
+  </si>
+  <si>
+    <t>royal_academy_engineering</t>
+  </si>
+  <si>
+    <t>royal_society</t>
+  </si>
+  <si>
+    <t>stfc</t>
+  </si>
+  <si>
+    <t>uk_space_agency</t>
+  </si>
+  <si>
+    <t>wellcome</t>
   </si>
   <si>
     <t>university of central lancashire</t>
@@ -1685,7 +1730,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:Y63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1693,7 +1738,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1721,1988 +1766,3055 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" s="1" t="n">
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
         <v>1761</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" t="s"/>
+      <c r="L2" t="s"/>
+      <c r="M2" t="s"/>
+      <c r="N2" t="s"/>
+      <c r="O2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="P2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="Q2" t="s"/>
+      <c r="R2" t="s"/>
+      <c r="S2" t="s"/>
+      <c r="T2" t="s"/>
+      <c r="U2" t="s"/>
+      <c r="V2" t="s"/>
+      <c r="W2" t="s"/>
+      <c r="X2" t="s"/>
+      <c r="Y2" t="s"/>
+    </row>
+    <row r="3" spans="1:25">
       <c r="A3" s="1" t="n">
-        <v>202</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>1956</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>39</v>
+      </c>
+      <c r="K3" t="s"/>
+      <c r="L3" t="s"/>
+      <c r="M3" t="s"/>
+      <c r="N3" t="s"/>
+      <c r="O3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" t="s"/>
+      <c r="Q3" t="s"/>
+      <c r="R3" t="s"/>
+      <c r="S3" t="s"/>
+      <c r="T3" t="s"/>
+      <c r="U3" t="s"/>
+      <c r="V3" t="s"/>
+      <c r="W3" t="s"/>
+      <c r="X3" t="s"/>
+      <c r="Y3" t="s"/>
+    </row>
+    <row r="4" spans="1:25">
       <c r="A4" s="1" t="n">
-        <v>203</v>
+        <v>2</v>
       </c>
       <c r="B4" t="n">
         <v>1957</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>47</v>
+      </c>
+      <c r="K4" t="s"/>
+      <c r="L4" t="s"/>
+      <c r="M4" t="s"/>
+      <c r="N4" t="s"/>
+      <c r="O4" t="s"/>
+      <c r="P4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" t="s"/>
+      <c r="R4" t="s"/>
+      <c r="S4" t="s"/>
+      <c r="T4" t="s"/>
+      <c r="U4" t="s"/>
+      <c r="V4" t="s"/>
+      <c r="W4" t="s"/>
+      <c r="X4" t="s"/>
+      <c r="Y4" t="s"/>
+    </row>
+    <row r="5" spans="1:25">
       <c r="A5" s="1" t="n">
-        <v>369</v>
+        <v>3</v>
       </c>
       <c r="B5" t="n">
         <v>3462</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="J5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>55</v>
+      </c>
+      <c r="K5" t="s"/>
+      <c r="L5" t="s"/>
+      <c r="M5" t="s"/>
+      <c r="N5" t="s"/>
+      <c r="O5" t="s"/>
+      <c r="P5" t="s"/>
+      <c r="Q5" t="s"/>
+      <c r="R5" t="s"/>
+      <c r="S5" t="s"/>
+      <c r="T5" t="s"/>
+      <c r="U5" t="s"/>
+      <c r="V5" t="s"/>
+      <c r="W5" t="s"/>
+      <c r="X5" t="s"/>
+      <c r="Y5" t="s"/>
+    </row>
+    <row r="6" spans="1:25">
       <c r="A6" s="1" t="n">
-        <v>524</v>
+        <v>4</v>
       </c>
       <c r="B6" t="n">
         <v>4138</v>
       </c>
       <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
         <v>41</v>
       </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>62</v>
+      </c>
+      <c r="K6" t="s"/>
+      <c r="L6" t="s"/>
+      <c r="M6" t="s"/>
+      <c r="N6" t="s"/>
+      <c r="O6" t="s"/>
+      <c r="P6" t="s"/>
+      <c r="Q6" t="s"/>
+      <c r="R6" t="s"/>
+      <c r="S6" t="s"/>
+      <c r="T6" t="s"/>
+      <c r="U6" t="s"/>
+      <c r="V6" t="s"/>
+      <c r="W6" t="s"/>
+      <c r="X6" t="s"/>
+      <c r="Y6" t="s"/>
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7" s="1" t="n">
-        <v>525</v>
+        <v>5</v>
       </c>
       <c r="B7" t="n">
         <v>4139</v>
       </c>
       <c r="C7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" t="s">
         <v>41</v>
       </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="H7" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="I7" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="J7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>68</v>
+      </c>
+      <c r="K7" t="s"/>
+      <c r="L7" t="s"/>
+      <c r="M7" t="s"/>
+      <c r="N7" t="s"/>
+      <c r="O7" t="s"/>
+      <c r="P7" t="s"/>
+      <c r="Q7" t="s"/>
+      <c r="R7" t="s"/>
+      <c r="S7" t="s"/>
+      <c r="T7" t="s"/>
+      <c r="U7" t="s"/>
+      <c r="V7" t="s"/>
+      <c r="W7" t="s"/>
+      <c r="X7" t="s"/>
+      <c r="Y7" t="s"/>
+    </row>
+    <row r="8" spans="1:25">
       <c r="A8" s="1" t="n">
-        <v>663</v>
+        <v>6</v>
       </c>
       <c r="B8" t="n">
         <v>4907</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="H8" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="I8" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="J8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>75</v>
+      </c>
+      <c r="K8" t="s"/>
+      <c r="L8" t="s"/>
+      <c r="M8" t="s"/>
+      <c r="N8" t="s"/>
+      <c r="O8" t="s"/>
+      <c r="P8" t="s"/>
+      <c r="Q8" t="s"/>
+      <c r="R8" t="s"/>
+      <c r="S8" t="s"/>
+      <c r="T8" t="s"/>
+      <c r="U8" t="s"/>
+      <c r="V8" t="s"/>
+      <c r="W8" t="s"/>
+      <c r="X8" t="s"/>
+      <c r="Y8" t="s"/>
+    </row>
+    <row r="9" spans="1:25">
       <c r="A9" s="1" t="n">
-        <v>683</v>
+        <v>7</v>
       </c>
       <c r="B9" t="n">
         <v>4959</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="I9" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="J9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>83</v>
+      </c>
+      <c r="K9" t="s"/>
+      <c r="L9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" t="s"/>
+      <c r="N9" t="s"/>
+      <c r="O9" t="s">
+        <v>13</v>
+      </c>
+      <c r="P9" t="s"/>
+      <c r="Q9" t="s"/>
+      <c r="R9" t="s"/>
+      <c r="S9" t="s"/>
+      <c r="T9" t="s">
+        <v>18</v>
+      </c>
+      <c r="U9" t="s"/>
+      <c r="V9" t="s">
+        <v>20</v>
+      </c>
+      <c r="W9" t="s">
+        <v>21</v>
+      </c>
+      <c r="X9" t="s"/>
+      <c r="Y9" t="s"/>
+    </row>
+    <row r="10" spans="1:25">
       <c r="A10" s="1" t="n">
-        <v>715</v>
+        <v>8</v>
       </c>
       <c r="B10" t="n">
         <v>5297</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="G10" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="H10" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="I10" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="J10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>90</v>
+      </c>
+      <c r="K10" t="s"/>
+      <c r="L10" t="s"/>
+      <c r="M10" t="s"/>
+      <c r="N10" t="s"/>
+      <c r="O10" t="s"/>
+      <c r="P10" t="s"/>
+      <c r="Q10" t="s"/>
+      <c r="R10" t="s"/>
+      <c r="S10" t="s"/>
+      <c r="T10" t="s"/>
+      <c r="U10" t="s"/>
+      <c r="V10" t="s"/>
+      <c r="W10" t="s"/>
+      <c r="X10" t="s"/>
+      <c r="Y10" t="s"/>
+    </row>
+    <row r="11" spans="1:25">
       <c r="A11" s="1" t="n">
-        <v>826</v>
+        <v>9</v>
       </c>
       <c r="B11" t="n">
         <v>6339</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="G11" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="H11" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="I11" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="J11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>97</v>
+      </c>
+      <c r="K11" t="s"/>
+      <c r="L11" t="s"/>
+      <c r="M11" t="s"/>
+      <c r="N11" t="s"/>
+      <c r="O11" t="s">
+        <v>13</v>
+      </c>
+      <c r="P11" t="s"/>
+      <c r="Q11" t="s"/>
+      <c r="R11" t="s"/>
+      <c r="S11" t="s"/>
+      <c r="T11" t="s"/>
+      <c r="U11" t="s"/>
+      <c r="V11" t="s"/>
+      <c r="W11" t="s"/>
+      <c r="X11" t="s"/>
+      <c r="Y11" t="s"/>
+    </row>
+    <row r="12" spans="1:25">
       <c r="A12" s="1" t="n">
-        <v>1088</v>
+        <v>10</v>
       </c>
       <c r="B12" t="n">
         <v>9501</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D12" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="E12" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="F12" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="G12" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="H12" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="I12" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="J12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>105</v>
+      </c>
+      <c r="K12" t="s"/>
+      <c r="L12" t="s"/>
+      <c r="M12" t="s"/>
+      <c r="N12" t="s"/>
+      <c r="O12" t="s">
+        <v>13</v>
+      </c>
+      <c r="P12" t="s"/>
+      <c r="Q12" t="s"/>
+      <c r="R12" t="s"/>
+      <c r="S12" t="s"/>
+      <c r="T12" t="s"/>
+      <c r="U12" t="s"/>
+      <c r="V12" t="s"/>
+      <c r="W12" t="s"/>
+      <c r="X12" t="s"/>
+      <c r="Y12" t="s"/>
+    </row>
+    <row r="13" spans="1:25">
       <c r="A13" s="1" t="n">
-        <v>1092</v>
+        <v>11</v>
       </c>
       <c r="B13" t="n">
         <v>9508</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="F13" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="G13" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="H13" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="I13" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="J13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>113</v>
+      </c>
+      <c r="K13" t="s"/>
+      <c r="L13" t="s"/>
+      <c r="M13" t="s"/>
+      <c r="N13" t="s"/>
+      <c r="O13" t="s"/>
+      <c r="P13" t="s"/>
+      <c r="Q13" t="s"/>
+      <c r="R13" t="s"/>
+      <c r="S13" t="s"/>
+      <c r="T13" t="s"/>
+      <c r="U13" t="s"/>
+      <c r="V13" t="s"/>
+      <c r="W13" t="s"/>
+      <c r="X13" t="s"/>
+      <c r="Y13" t="s"/>
+    </row>
+    <row r="14" spans="1:25">
       <c r="A14" s="1" t="n">
-        <v>1152</v>
+        <v>12</v>
       </c>
       <c r="B14" t="n">
         <v>11775</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="F14" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="G14" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="H14" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="I14" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="J14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>120</v>
+      </c>
+      <c r="K14" t="s"/>
+      <c r="L14" t="s"/>
+      <c r="M14" t="s"/>
+      <c r="N14" t="s"/>
+      <c r="O14" t="s">
+        <v>13</v>
+      </c>
+      <c r="P14" t="s"/>
+      <c r="Q14" t="s"/>
+      <c r="R14" t="s"/>
+      <c r="S14" t="s"/>
+      <c r="T14" t="s"/>
+      <c r="U14" t="s"/>
+      <c r="V14" t="s"/>
+      <c r="W14" t="s"/>
+      <c r="X14" t="s"/>
+      <c r="Y14" t="s"/>
+    </row>
+    <row r="15" spans="1:25">
       <c r="A15" s="1" t="n">
-        <v>1157</v>
+        <v>13</v>
       </c>
       <c r="B15" t="n">
         <v>11780</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="F15" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="G15" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="H15" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="I15" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="J15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>127</v>
+      </c>
+      <c r="K15" t="s"/>
+      <c r="L15" t="s"/>
+      <c r="M15" t="s"/>
+      <c r="N15" t="s"/>
+      <c r="O15" t="s"/>
+      <c r="P15" t="s"/>
+      <c r="Q15" t="s"/>
+      <c r="R15" t="s"/>
+      <c r="S15" t="s"/>
+      <c r="T15" t="s"/>
+      <c r="U15" t="s"/>
+      <c r="V15" t="s"/>
+      <c r="W15" t="s"/>
+      <c r="X15" t="s"/>
+      <c r="Y15" t="s"/>
+    </row>
+    <row r="16" spans="1:25">
       <c r="A16" s="1" t="n">
-        <v>1315</v>
+        <v>14</v>
       </c>
       <c r="B16" t="n">
         <v>12998</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="F16" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="G16" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="H16" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="I16" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="J16" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>134</v>
+      </c>
+      <c r="K16" t="s"/>
+      <c r="L16" t="s"/>
+      <c r="M16" t="s"/>
+      <c r="N16" t="s"/>
+      <c r="O16" t="s"/>
+      <c r="P16" t="s"/>
+      <c r="Q16" t="s"/>
+      <c r="R16" t="s"/>
+      <c r="S16" t="s"/>
+      <c r="T16" t="s"/>
+      <c r="U16" t="s"/>
+      <c r="V16" t="s"/>
+      <c r="W16" t="s"/>
+      <c r="X16" t="s"/>
+      <c r="Y16" t="s"/>
+    </row>
+    <row r="17" spans="1:25">
       <c r="A17" s="1" t="n">
-        <v>1345</v>
+        <v>15</v>
       </c>
       <c r="B17" t="n">
         <v>13783</v>
       </c>
       <c r="C17" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="F17" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="G17" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="H17" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="I17" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="J17" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>141</v>
+      </c>
+      <c r="K17" t="s"/>
+      <c r="L17" t="s"/>
+      <c r="M17" t="s"/>
+      <c r="N17" t="s"/>
+      <c r="O17" t="s">
+        <v>13</v>
+      </c>
+      <c r="P17" t="s"/>
+      <c r="Q17" t="s"/>
+      <c r="R17" t="s"/>
+      <c r="S17" t="s"/>
+      <c r="T17" t="s"/>
+      <c r="U17" t="s"/>
+      <c r="V17" t="s"/>
+      <c r="W17" t="s"/>
+      <c r="X17" t="s"/>
+      <c r="Y17" t="s"/>
+    </row>
+    <row r="18" spans="1:25">
       <c r="A18" s="1" t="n">
-        <v>1423</v>
+        <v>16</v>
       </c>
       <c r="B18" t="n">
         <v>14576</v>
       </c>
       <c r="C18" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="F18" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="G18" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="H18" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="I18" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="J18" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>148</v>
+      </c>
+      <c r="K18" t="s"/>
+      <c r="L18" t="s"/>
+      <c r="M18" t="s"/>
+      <c r="N18" t="s"/>
+      <c r="O18" t="s"/>
+      <c r="P18" t="s"/>
+      <c r="Q18" t="s"/>
+      <c r="R18" t="s"/>
+      <c r="S18" t="s"/>
+      <c r="T18" t="s"/>
+      <c r="U18" t="s"/>
+      <c r="V18" t="s"/>
+      <c r="W18" t="s">
+        <v>21</v>
+      </c>
+      <c r="X18" t="s"/>
+      <c r="Y18" t="s"/>
+    </row>
+    <row r="19" spans="1:25">
       <c r="A19" s="1" t="n">
-        <v>1431</v>
+        <v>17</v>
       </c>
       <c r="B19" t="n">
         <v>14585</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D19" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="E19" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="F19" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="G19" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="H19" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="I19" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="J19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>155</v>
+      </c>
+      <c r="K19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" t="s"/>
+      <c r="M19" t="s"/>
+      <c r="N19" t="s"/>
+      <c r="O19" t="s"/>
+      <c r="P19" t="s"/>
+      <c r="Q19" t="s"/>
+      <c r="R19" t="s">
+        <v>16</v>
+      </c>
+      <c r="S19" t="s"/>
+      <c r="T19" t="s"/>
+      <c r="U19" t="s"/>
+      <c r="V19" t="s"/>
+      <c r="W19" t="s"/>
+      <c r="X19" t="s"/>
+      <c r="Y19" t="s"/>
+    </row>
+    <row r="20" spans="1:25">
       <c r="A20" s="1" t="n">
-        <v>1446</v>
+        <v>18</v>
       </c>
       <c r="B20" t="n">
         <v>14713</v>
       </c>
       <c r="C20" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="D20" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="E20" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="F20" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="G20" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="H20" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="I20" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="J20" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>163</v>
+      </c>
+      <c r="K20" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" t="s"/>
+      <c r="M20" t="s"/>
+      <c r="N20" t="s"/>
+      <c r="O20" t="s"/>
+      <c r="P20" t="s"/>
+      <c r="Q20" t="s"/>
+      <c r="R20" t="s"/>
+      <c r="S20" t="s"/>
+      <c r="T20" t="s"/>
+      <c r="U20" t="s"/>
+      <c r="V20" t="s"/>
+      <c r="W20" t="s"/>
+      <c r="X20" t="s"/>
+      <c r="Y20" t="s"/>
+    </row>
+    <row r="21" spans="1:25">
       <c r="A21" s="1" t="n">
-        <v>1554</v>
+        <v>19</v>
       </c>
       <c r="B21" t="n">
         <v>16697</v>
       </c>
       <c r="C21" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="F21" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="G21" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="H21" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="I21" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="J21" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+        <v>169</v>
+      </c>
+      <c r="K21" t="s"/>
+      <c r="L21" t="s"/>
+      <c r="M21" t="s"/>
+      <c r="N21" t="s"/>
+      <c r="O21" t="s">
+        <v>13</v>
+      </c>
+      <c r="P21" t="s"/>
+      <c r="Q21" t="s"/>
+      <c r="R21" t="s"/>
+      <c r="S21" t="s">
+        <v>17</v>
+      </c>
+      <c r="T21" t="s"/>
+      <c r="U21" t="s"/>
+      <c r="V21" t="s">
+        <v>20</v>
+      </c>
+      <c r="W21" t="s"/>
+      <c r="X21" t="s"/>
+      <c r="Y21" t="s"/>
+    </row>
+    <row r="22" spans="1:25">
       <c r="A22" s="1" t="n">
-        <v>1825</v>
+        <v>20</v>
       </c>
       <c r="B22" t="n">
         <v>18590</v>
       </c>
       <c r="C22" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E22" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="F22" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="G22" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="H22" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="I22" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="J22" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+        <v>176</v>
+      </c>
+      <c r="K22" t="s"/>
+      <c r="L22" t="s"/>
+      <c r="M22" t="s"/>
+      <c r="N22" t="s"/>
+      <c r="O22" t="s">
+        <v>13</v>
+      </c>
+      <c r="P22" t="s"/>
+      <c r="Q22" t="s"/>
+      <c r="R22" t="s"/>
+      <c r="S22" t="s"/>
+      <c r="T22" t="s"/>
+      <c r="U22" t="s">
+        <v>19</v>
+      </c>
+      <c r="V22" t="s"/>
+      <c r="W22" t="s"/>
+      <c r="X22" t="s"/>
+      <c r="Y22" t="s"/>
+    </row>
+    <row r="23" spans="1:25">
       <c r="A23" s="1" t="n">
-        <v>1954</v>
+        <v>21</v>
       </c>
       <c r="B23" t="n">
         <v>19859</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="F23" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="G23" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="H23" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="I23" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="J23" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <v>182</v>
+      </c>
+      <c r="K23" t="s"/>
+      <c r="L23" t="s"/>
+      <c r="M23" t="s"/>
+      <c r="N23" t="s"/>
+      <c r="O23" t="s"/>
+      <c r="P23" t="s"/>
+      <c r="Q23" t="s"/>
+      <c r="R23" t="s"/>
+      <c r="S23" t="s"/>
+      <c r="T23" t="s"/>
+      <c r="U23" t="s"/>
+      <c r="V23" t="s"/>
+      <c r="W23" t="s"/>
+      <c r="X23" t="s"/>
+      <c r="Y23" t="s"/>
+    </row>
+    <row r="24" spans="1:25">
       <c r="A24" s="1" t="n">
-        <v>1973</v>
+        <v>22</v>
       </c>
       <c r="B24" t="n">
         <v>19994</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E24" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="F24" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="G24" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="H24" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="I24" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="J24" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+        <v>188</v>
+      </c>
+      <c r="K24" t="s"/>
+      <c r="L24" t="s"/>
+      <c r="M24" t="s"/>
+      <c r="N24" t="s"/>
+      <c r="O24" t="s">
+        <v>13</v>
+      </c>
+      <c r="P24" t="s"/>
+      <c r="Q24" t="s"/>
+      <c r="R24" t="s"/>
+      <c r="S24" t="s"/>
+      <c r="T24" t="s"/>
+      <c r="U24" t="s"/>
+      <c r="V24" t="s"/>
+      <c r="W24" t="s"/>
+      <c r="X24" t="s"/>
+      <c r="Y24" t="s"/>
+    </row>
+    <row r="25" spans="1:25">
       <c r="A25" s="1" t="n">
-        <v>1992</v>
+        <v>23</v>
       </c>
       <c r="B25" t="n">
         <v>20085</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E25" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="F25" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="G25" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="H25" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="I25" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="J25" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+        <v>194</v>
+      </c>
+      <c r="K25" t="s"/>
+      <c r="L25" t="s"/>
+      <c r="M25" t="s"/>
+      <c r="N25" t="s"/>
+      <c r="O25" t="s">
+        <v>13</v>
+      </c>
+      <c r="P25" t="s"/>
+      <c r="Q25" t="s"/>
+      <c r="R25" t="s"/>
+      <c r="S25" t="s"/>
+      <c r="T25" t="s"/>
+      <c r="U25" t="s"/>
+      <c r="V25" t="s"/>
+      <c r="W25" t="s"/>
+      <c r="X25" t="s"/>
+      <c r="Y25" t="s"/>
+    </row>
+    <row r="26" spans="1:25">
       <c r="A26" s="1" t="n">
-        <v>2005</v>
+        <v>24</v>
       </c>
       <c r="B26" t="n">
         <v>20286</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E26" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="F26" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="G26" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="H26" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="I26" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="J26" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+        <v>201</v>
+      </c>
+      <c r="K26" t="s"/>
+      <c r="L26" t="s"/>
+      <c r="M26" t="s"/>
+      <c r="N26" t="s"/>
+      <c r="O26" t="s"/>
+      <c r="P26" t="s"/>
+      <c r="Q26" t="s"/>
+      <c r="R26" t="s"/>
+      <c r="S26" t="s"/>
+      <c r="T26" t="s"/>
+      <c r="U26" t="s"/>
+      <c r="V26" t="s"/>
+      <c r="W26" t="s"/>
+      <c r="X26" t="s"/>
+      <c r="Y26" t="s"/>
+    </row>
+    <row r="27" spans="1:25">
       <c r="A27" s="1" t="n">
-        <v>2010</v>
+        <v>25</v>
       </c>
       <c r="B27" t="n">
         <v>20329</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D27" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E27" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="F27" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="G27" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="H27" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="I27" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="J27" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+        <v>207</v>
+      </c>
+      <c r="K27" t="s"/>
+      <c r="L27" t="s"/>
+      <c r="M27" t="s"/>
+      <c r="N27" t="s"/>
+      <c r="O27" t="s"/>
+      <c r="P27" t="s"/>
+      <c r="Q27" t="s"/>
+      <c r="R27" t="s"/>
+      <c r="S27" t="s"/>
+      <c r="T27" t="s"/>
+      <c r="U27" t="s"/>
+      <c r="V27" t="s"/>
+      <c r="W27" t="s"/>
+      <c r="X27" t="s"/>
+      <c r="Y27" t="s"/>
+    </row>
+    <row r="28" spans="1:25">
       <c r="A28" s="1" t="n">
-        <v>2034</v>
+        <v>26</v>
       </c>
       <c r="B28" t="n">
         <v>20514</v>
       </c>
       <c r="C28" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="D28" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E28" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="F28" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="G28" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="H28" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="I28" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="J28" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+        <v>214</v>
+      </c>
+      <c r="K28" t="s"/>
+      <c r="L28" t="s"/>
+      <c r="M28" t="s"/>
+      <c r="N28" t="s"/>
+      <c r="O28" t="s"/>
+      <c r="P28" t="s"/>
+      <c r="Q28" t="s"/>
+      <c r="R28" t="s"/>
+      <c r="S28" t="s"/>
+      <c r="T28" t="s"/>
+      <c r="U28" t="s"/>
+      <c r="V28" t="s"/>
+      <c r="W28" t="s"/>
+      <c r="X28" t="s"/>
+      <c r="Y28" t="s"/>
+    </row>
+    <row r="29" spans="1:25">
       <c r="A29" s="1" t="n">
-        <v>2107</v>
+        <v>27</v>
       </c>
       <c r="B29" t="n">
         <v>21273</v>
       </c>
       <c r="C29" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="D29" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E29" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="F29" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="G29" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="H29" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="I29" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="J29" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+        <v>221</v>
+      </c>
+      <c r="K29" t="s"/>
+      <c r="L29" t="s"/>
+      <c r="M29" t="s"/>
+      <c r="N29" t="s"/>
+      <c r="O29" t="s">
+        <v>13</v>
+      </c>
+      <c r="P29" t="s"/>
+      <c r="Q29" t="s"/>
+      <c r="R29" t="s"/>
+      <c r="S29" t="s"/>
+      <c r="T29" t="s"/>
+      <c r="U29" t="s"/>
+      <c r="V29" t="s"/>
+      <c r="W29" t="s"/>
+      <c r="X29" t="s"/>
+      <c r="Y29" t="s"/>
+    </row>
+    <row r="30" spans="1:25">
       <c r="A30" s="1" t="n">
-        <v>2410</v>
+        <v>28</v>
       </c>
       <c r="B30" t="n">
         <v>23622</v>
       </c>
       <c r="C30" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="D30" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="E30" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="F30" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="G30" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="H30" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="I30" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="J30" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+        <v>228</v>
+      </c>
+      <c r="K30" t="s"/>
+      <c r="L30" t="s">
+        <v>10</v>
+      </c>
+      <c r="M30" t="s"/>
+      <c r="N30" t="s"/>
+      <c r="O30" t="s"/>
+      <c r="P30" t="s"/>
+      <c r="Q30" t="s">
+        <v>15</v>
+      </c>
+      <c r="R30" t="s"/>
+      <c r="S30" t="s"/>
+      <c r="T30" t="s"/>
+      <c r="U30" t="s"/>
+      <c r="V30" t="s"/>
+      <c r="W30" t="s"/>
+      <c r="X30" t="s"/>
+      <c r="Y30" t="s"/>
+    </row>
+    <row r="31" spans="1:25">
       <c r="A31" s="1" t="n">
-        <v>2472</v>
+        <v>29</v>
       </c>
       <c r="B31" t="n">
         <v>23898</v>
       </c>
       <c r="C31" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="D31" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="E31" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="F31" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="G31" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="H31" t="s">
-        <v>218</v>
+        <v>233</v>
       </c>
       <c r="I31" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="J31" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+        <v>235</v>
+      </c>
+      <c r="K31" t="s"/>
+      <c r="L31" t="s"/>
+      <c r="M31" t="s"/>
+      <c r="N31" t="s"/>
+      <c r="O31" t="s"/>
+      <c r="P31" t="s"/>
+      <c r="Q31" t="s"/>
+      <c r="R31" t="s"/>
+      <c r="S31" t="s"/>
+      <c r="T31" t="s"/>
+      <c r="U31" t="s"/>
+      <c r="V31" t="s"/>
+      <c r="W31" t="s"/>
+      <c r="X31" t="s"/>
+      <c r="Y31" t="s"/>
+    </row>
+    <row r="32" spans="1:25">
       <c r="A32" s="1" t="n">
-        <v>2508</v>
+        <v>30</v>
       </c>
       <c r="B32" t="n">
         <v>23934</v>
       </c>
       <c r="C32" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="D32" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E32" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="F32" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="G32" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="H32" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="I32" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
       <c r="J32" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+        <v>242</v>
+      </c>
+      <c r="K32" t="s"/>
+      <c r="L32" t="s"/>
+      <c r="M32" t="s"/>
+      <c r="N32" t="s"/>
+      <c r="O32" t="s">
+        <v>13</v>
+      </c>
+      <c r="P32" t="s"/>
+      <c r="Q32" t="s"/>
+      <c r="R32" t="s"/>
+      <c r="S32" t="s"/>
+      <c r="T32" t="s"/>
+      <c r="U32" t="s"/>
+      <c r="V32" t="s"/>
+      <c r="W32" t="s">
+        <v>21</v>
+      </c>
+      <c r="X32" t="s"/>
+      <c r="Y32" t="s"/>
+    </row>
+    <row r="33" spans="1:25">
       <c r="A33" s="1" t="n">
-        <v>2514</v>
+        <v>31</v>
       </c>
       <c r="B33" t="n">
         <v>23940</v>
       </c>
       <c r="C33" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="D33" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E33" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="F33" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
       <c r="G33" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="H33" t="s">
-        <v>231</v>
+        <v>246</v>
       </c>
       <c r="I33" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="J33" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
+        <v>248</v>
+      </c>
+      <c r="K33" t="s"/>
+      <c r="L33" t="s"/>
+      <c r="M33" t="s"/>
+      <c r="N33" t="s"/>
+      <c r="O33" t="s">
+        <v>13</v>
+      </c>
+      <c r="P33" t="s"/>
+      <c r="Q33" t="s"/>
+      <c r="R33" t="s"/>
+      <c r="S33" t="s"/>
+      <c r="T33" t="s"/>
+      <c r="U33" t="s"/>
+      <c r="V33" t="s"/>
+      <c r="W33" t="s"/>
+      <c r="X33" t="s"/>
+      <c r="Y33" t="s"/>
+    </row>
+    <row r="34" spans="1:25">
       <c r="A34" s="1" t="n">
-        <v>2724</v>
+        <v>32</v>
       </c>
       <c r="B34" t="n">
         <v>25860</v>
       </c>
       <c r="C34" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="D34" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E34" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="F34" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="G34" t="s">
-        <v>237</v>
+        <v>252</v>
       </c>
       <c r="H34" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="I34" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="J34" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
+        <v>255</v>
+      </c>
+      <c r="K34" t="s"/>
+      <c r="L34" t="s"/>
+      <c r="M34" t="s"/>
+      <c r="N34" t="s"/>
+      <c r="O34" t="s">
+        <v>13</v>
+      </c>
+      <c r="P34" t="s"/>
+      <c r="Q34" t="s"/>
+      <c r="R34" t="s"/>
+      <c r="S34" t="s"/>
+      <c r="T34" t="s"/>
+      <c r="U34" t="s"/>
+      <c r="V34" t="s">
+        <v>20</v>
+      </c>
+      <c r="W34" t="s"/>
+      <c r="X34" t="s"/>
+      <c r="Y34" t="s"/>
+    </row>
+    <row r="35" spans="1:25">
       <c r="A35" s="1" t="n">
-        <v>2743</v>
+        <v>33</v>
       </c>
       <c r="B35" t="n">
         <v>26132</v>
       </c>
       <c r="C35" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="D35" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E35" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="F35" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="G35" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="H35" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="I35" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
       <c r="J35" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
+        <v>262</v>
+      </c>
+      <c r="K35" t="s"/>
+      <c r="L35" t="s"/>
+      <c r="M35" t="s"/>
+      <c r="N35" t="s"/>
+      <c r="O35" t="s"/>
+      <c r="P35" t="s"/>
+      <c r="Q35" t="s"/>
+      <c r="R35" t="s"/>
+      <c r="S35" t="s"/>
+      <c r="T35" t="s"/>
+      <c r="U35" t="s"/>
+      <c r="V35" t="s"/>
+      <c r="W35" t="s"/>
+      <c r="X35" t="s"/>
+      <c r="Y35" t="s"/>
+    </row>
+    <row r="36" spans="1:25">
       <c r="A36" s="1" t="n">
-        <v>2747</v>
+        <v>34</v>
       </c>
       <c r="B36" t="n">
         <v>26263</v>
       </c>
       <c r="C36" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="D36" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E36" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="F36" t="s">
-        <v>249</v>
+        <v>264</v>
       </c>
       <c r="G36" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="H36" t="s">
-        <v>251</v>
+        <v>266</v>
       </c>
       <c r="I36" t="s">
-        <v>252</v>
+        <v>267</v>
       </c>
       <c r="J36" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
+        <v>268</v>
+      </c>
+      <c r="K36" t="s"/>
+      <c r="L36" t="s"/>
+      <c r="M36" t="s"/>
+      <c r="N36" t="s"/>
+      <c r="O36" t="s">
+        <v>13</v>
+      </c>
+      <c r="P36" t="s"/>
+      <c r="Q36" t="s"/>
+      <c r="R36" t="s"/>
+      <c r="S36" t="s"/>
+      <c r="T36" t="s"/>
+      <c r="U36" t="s"/>
+      <c r="V36" t="s"/>
+      <c r="W36" t="s"/>
+      <c r="X36" t="s"/>
+      <c r="Y36" t="s"/>
+    </row>
+    <row r="37" spans="1:25">
       <c r="A37" s="1" t="n">
-        <v>2947</v>
+        <v>35</v>
       </c>
       <c r="B37" t="n">
         <v>28097</v>
       </c>
       <c r="C37" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
       <c r="D37" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="E37" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
       <c r="F37" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="G37" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="H37" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="I37" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="J37" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
+        <v>276</v>
+      </c>
+      <c r="K37" t="s"/>
+      <c r="L37" t="s"/>
+      <c r="M37" t="s"/>
+      <c r="N37" t="s"/>
+      <c r="O37" t="s"/>
+      <c r="P37" t="s"/>
+      <c r="Q37" t="s"/>
+      <c r="R37" t="s"/>
+      <c r="S37" t="s"/>
+      <c r="T37" t="s"/>
+      <c r="U37" t="s"/>
+      <c r="V37" t="s"/>
+      <c r="W37" t="s"/>
+      <c r="X37" t="s"/>
+      <c r="Y37" t="s"/>
+    </row>
+    <row r="38" spans="1:25">
       <c r="A38" s="1" t="n">
-        <v>2987</v>
+        <v>36</v>
       </c>
       <c r="B38" t="n">
         <v>28137</v>
       </c>
       <c r="C38" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="D38" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E38" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="F38" t="s">
-        <v>264</v>
+        <v>279</v>
       </c>
       <c r="G38" t="s">
-        <v>265</v>
+        <v>280</v>
       </c>
       <c r="H38" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="I38" t="s">
-        <v>267</v>
+        <v>282</v>
       </c>
       <c r="J38" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
+        <v>283</v>
+      </c>
+      <c r="K38" t="s"/>
+      <c r="L38" t="s"/>
+      <c r="M38" t="s"/>
+      <c r="N38" t="s"/>
+      <c r="O38" t="s"/>
+      <c r="P38" t="s"/>
+      <c r="Q38" t="s"/>
+      <c r="R38" t="s"/>
+      <c r="S38" t="s"/>
+      <c r="T38" t="s"/>
+      <c r="U38" t="s"/>
+      <c r="V38" t="s"/>
+      <c r="W38" t="s"/>
+      <c r="X38" t="s"/>
+      <c r="Y38" t="s"/>
+    </row>
+    <row r="39" spans="1:25">
       <c r="A39" s="1" t="n">
-        <v>2988</v>
+        <v>37</v>
       </c>
       <c r="B39" t="n">
         <v>28138</v>
       </c>
       <c r="C39" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="D39" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E39" t="s">
-        <v>269</v>
+        <v>284</v>
       </c>
       <c r="F39" t="s">
-        <v>270</v>
+        <v>285</v>
       </c>
       <c r="G39" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="H39" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="I39" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
       <c r="J39" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
+        <v>289</v>
+      </c>
+      <c r="K39" t="s"/>
+      <c r="L39" t="s"/>
+      <c r="M39" t="s"/>
+      <c r="N39" t="s"/>
+      <c r="O39" t="s"/>
+      <c r="P39" t="s"/>
+      <c r="Q39" t="s"/>
+      <c r="R39" t="s"/>
+      <c r="S39" t="s"/>
+      <c r="T39" t="s"/>
+      <c r="U39" t="s"/>
+      <c r="V39" t="s"/>
+      <c r="W39" t="s"/>
+      <c r="X39" t="s"/>
+      <c r="Y39" t="s"/>
+    </row>
+    <row r="40" spans="1:25">
       <c r="A40" s="1" t="n">
-        <v>3027</v>
+        <v>38</v>
       </c>
       <c r="B40" t="n">
         <v>28177</v>
       </c>
       <c r="C40" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="D40" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E40" t="s">
-        <v>276</v>
+        <v>291</v>
       </c>
       <c r="F40" t="s">
-        <v>277</v>
+        <v>292</v>
       </c>
       <c r="G40" t="s">
-        <v>278</v>
+        <v>293</v>
       </c>
       <c r="H40" t="s">
-        <v>279</v>
+        <v>294</v>
       </c>
       <c r="I40" t="s">
-        <v>280</v>
+        <v>295</v>
       </c>
       <c r="J40" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
+        <v>296</v>
+      </c>
+      <c r="K40" t="s"/>
+      <c r="L40" t="s"/>
+      <c r="M40" t="s"/>
+      <c r="N40" t="s"/>
+      <c r="O40" t="s"/>
+      <c r="P40" t="s"/>
+      <c r="Q40" t="s"/>
+      <c r="R40" t="s"/>
+      <c r="S40" t="s"/>
+      <c r="T40" t="s"/>
+      <c r="U40" t="s"/>
+      <c r="V40" t="s"/>
+      <c r="W40" t="s"/>
+      <c r="X40" t="s"/>
+      <c r="Y40" t="s"/>
+    </row>
+    <row r="41" spans="1:25">
       <c r="A41" s="1" t="n">
-        <v>3150</v>
+        <v>39</v>
       </c>
       <c r="B41" t="n">
         <v>28884</v>
       </c>
       <c r="C41" t="s">
-        <v>282</v>
+        <v>297</v>
       </c>
       <c r="D41" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="E41" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="F41" t="s">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="G41" t="s">
-        <v>286</v>
+        <v>301</v>
       </c>
       <c r="H41" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="I41" t="s">
-        <v>288</v>
+        <v>303</v>
       </c>
       <c r="J41" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
+        <v>304</v>
+      </c>
+      <c r="K41" t="s"/>
+      <c r="L41" t="s"/>
+      <c r="M41" t="s"/>
+      <c r="N41" t="s"/>
+      <c r="O41" t="s"/>
+      <c r="P41" t="s"/>
+      <c r="Q41" t="s"/>
+      <c r="R41" t="s"/>
+      <c r="S41" t="s"/>
+      <c r="T41" t="s"/>
+      <c r="U41" t="s"/>
+      <c r="V41" t="s"/>
+      <c r="W41" t="s"/>
+      <c r="X41" t="s"/>
+      <c r="Y41" t="s"/>
+    </row>
+    <row r="42" spans="1:25">
       <c r="A42" s="1" t="n">
-        <v>3265</v>
+        <v>40</v>
       </c>
       <c r="B42" t="n">
         <v>30149</v>
       </c>
       <c r="C42" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="D42" t="s">
-        <v>290</v>
+        <v>305</v>
       </c>
       <c r="E42" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F42" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="G42" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="H42" t="s">
-        <v>294</v>
+        <v>309</v>
       </c>
       <c r="I42" t="s">
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="J42" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
+        <v>311</v>
+      </c>
+      <c r="K42" t="s"/>
+      <c r="L42" t="s"/>
+      <c r="M42" t="s"/>
+      <c r="N42" t="s"/>
+      <c r="O42" t="s"/>
+      <c r="P42" t="s"/>
+      <c r="Q42" t="s"/>
+      <c r="R42" t="s"/>
+      <c r="S42" t="s"/>
+      <c r="T42" t="s"/>
+      <c r="U42" t="s"/>
+      <c r="V42" t="s"/>
+      <c r="W42" t="s"/>
+      <c r="X42" t="s"/>
+      <c r="Y42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25">
       <c r="A43" s="1" t="n">
-        <v>3842</v>
+        <v>41</v>
       </c>
       <c r="B43" t="n">
         <v>35580</v>
       </c>
       <c r="C43" t="s">
-        <v>297</v>
+        <v>312</v>
       </c>
       <c r="D43" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E43" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="F43" t="s">
-        <v>299</v>
+        <v>314</v>
       </c>
       <c r="G43" t="s">
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="H43" t="s">
-        <v>301</v>
+        <v>316</v>
       </c>
       <c r="I43" t="s">
-        <v>302</v>
+        <v>317</v>
       </c>
       <c r="J43" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
+        <v>318</v>
+      </c>
+      <c r="K43" t="s"/>
+      <c r="L43" t="s"/>
+      <c r="M43" t="s"/>
+      <c r="N43" t="s"/>
+      <c r="O43" t="s">
+        <v>13</v>
+      </c>
+      <c r="P43" t="s"/>
+      <c r="Q43" t="s"/>
+      <c r="R43" t="s"/>
+      <c r="S43" t="s"/>
+      <c r="T43" t="s"/>
+      <c r="U43" t="s"/>
+      <c r="V43" t="s">
+        <v>20</v>
+      </c>
+      <c r="W43" t="s"/>
+      <c r="X43" t="s"/>
+      <c r="Y43" t="s"/>
+    </row>
+    <row r="44" spans="1:25">
       <c r="A44" s="1" t="n">
-        <v>3884</v>
+        <v>42</v>
       </c>
       <c r="B44" t="n">
         <v>35831</v>
       </c>
       <c r="C44" t="s">
-        <v>304</v>
+        <v>319</v>
       </c>
       <c r="D44" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E44" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
       <c r="F44" t="s">
-        <v>306</v>
+        <v>321</v>
       </c>
       <c r="G44" t="s">
-        <v>307</v>
+        <v>322</v>
       </c>
       <c r="H44" t="s">
-        <v>308</v>
+        <v>323</v>
       </c>
       <c r="I44" t="s">
-        <v>309</v>
+        <v>324</v>
       </c>
       <c r="J44" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
+        <v>325</v>
+      </c>
+      <c r="K44" t="s"/>
+      <c r="L44" t="s"/>
+      <c r="M44" t="s"/>
+      <c r="N44" t="s"/>
+      <c r="O44" t="s">
+        <v>13</v>
+      </c>
+      <c r="P44" t="s"/>
+      <c r="Q44" t="s"/>
+      <c r="R44" t="s"/>
+      <c r="S44" t="s"/>
+      <c r="T44" t="s"/>
+      <c r="U44" t="s"/>
+      <c r="V44" t="s">
+        <v>20</v>
+      </c>
+      <c r="W44" t="s"/>
+      <c r="X44" t="s"/>
+      <c r="Y44" t="s"/>
+    </row>
+    <row r="45" spans="1:25">
       <c r="A45" s="1" t="n">
-        <v>4068</v>
+        <v>43</v>
       </c>
       <c r="B45" t="n">
         <v>37236</v>
       </c>
       <c r="C45" t="s">
-        <v>311</v>
+        <v>326</v>
       </c>
       <c r="D45" t="s">
-        <v>312</v>
+        <v>327</v>
       </c>
       <c r="E45" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
       <c r="F45" t="s">
-        <v>314</v>
+        <v>329</v>
       </c>
       <c r="G45" t="s">
-        <v>315</v>
+        <v>330</v>
       </c>
       <c r="H45" t="s">
-        <v>316</v>
+        <v>331</v>
       </c>
       <c r="I45" t="s">
-        <v>317</v>
+        <v>332</v>
       </c>
       <c r="J45" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
+        <v>333</v>
+      </c>
+      <c r="K45" t="s"/>
+      <c r="L45" t="s"/>
+      <c r="M45" t="s"/>
+      <c r="N45" t="s"/>
+      <c r="O45" t="s"/>
+      <c r="P45" t="s"/>
+      <c r="Q45" t="s"/>
+      <c r="R45" t="s"/>
+      <c r="S45" t="s"/>
+      <c r="T45" t="s"/>
+      <c r="U45" t="s"/>
+      <c r="V45" t="s"/>
+      <c r="W45" t="s"/>
+      <c r="X45" t="s"/>
+      <c r="Y45" t="s"/>
+    </row>
+    <row r="46" spans="1:25">
       <c r="A46" s="1" t="n">
-        <v>4504</v>
+        <v>44</v>
       </c>
       <c r="B46" t="n">
         <v>39427</v>
       </c>
       <c r="C46" t="s">
-        <v>319</v>
+        <v>334</v>
       </c>
       <c r="D46" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E46" t="s">
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="F46" t="s">
-        <v>321</v>
+        <v>336</v>
       </c>
       <c r="G46" t="s">
-        <v>322</v>
+        <v>337</v>
       </c>
       <c r="H46" t="s">
-        <v>323</v>
+        <v>338</v>
       </c>
       <c r="I46" t="s">
-        <v>324</v>
+        <v>339</v>
       </c>
       <c r="J46" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
+        <v>340</v>
+      </c>
+      <c r="K46" t="s"/>
+      <c r="L46" t="s"/>
+      <c r="M46" t="s"/>
+      <c r="N46" t="s"/>
+      <c r="O46" t="s"/>
+      <c r="P46" t="s"/>
+      <c r="Q46" t="s"/>
+      <c r="R46" t="s"/>
+      <c r="S46" t="s"/>
+      <c r="T46" t="s"/>
+      <c r="U46" t="s"/>
+      <c r="V46" t="s"/>
+      <c r="W46" t="s"/>
+      <c r="X46" t="s"/>
+      <c r="Y46" t="s"/>
+    </row>
+    <row r="47" spans="1:25">
       <c r="A47" s="1" t="n">
-        <v>4771</v>
+        <v>45</v>
       </c>
       <c r="B47" t="n">
         <v>40380</v>
       </c>
       <c r="C47" t="s">
-        <v>326</v>
+        <v>341</v>
       </c>
       <c r="D47" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E47" t="s">
-        <v>327</v>
+        <v>342</v>
       </c>
       <c r="F47" t="s">
-        <v>328</v>
+        <v>343</v>
       </c>
       <c r="G47" t="s">
-        <v>329</v>
+        <v>344</v>
       </c>
       <c r="H47" t="s">
-        <v>330</v>
+        <v>345</v>
       </c>
       <c r="I47" t="s">
-        <v>331</v>
+        <v>346</v>
       </c>
       <c r="J47" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
+        <v>347</v>
+      </c>
+      <c r="K47" t="s"/>
+      <c r="L47" t="s"/>
+      <c r="M47" t="s"/>
+      <c r="N47" t="s"/>
+      <c r="O47" t="s"/>
+      <c r="P47" t="s"/>
+      <c r="Q47" t="s"/>
+      <c r="R47" t="s"/>
+      <c r="S47" t="s"/>
+      <c r="T47" t="s"/>
+      <c r="U47" t="s"/>
+      <c r="V47" t="s"/>
+      <c r="W47" t="s"/>
+      <c r="X47" t="s"/>
+      <c r="Y47" t="s"/>
+    </row>
+    <row r="48" spans="1:25">
       <c r="A48" s="1" t="n">
-        <v>4964</v>
+        <v>46</v>
       </c>
       <c r="B48" t="n">
         <v>41138</v>
       </c>
       <c r="C48" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="D48" t="s">
-        <v>290</v>
+        <v>305</v>
       </c>
       <c r="E48" t="s">
-        <v>333</v>
+        <v>348</v>
       </c>
       <c r="F48" t="s">
-        <v>334</v>
+        <v>349</v>
       </c>
       <c r="G48" t="s">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="H48" t="s">
-        <v>336</v>
+        <v>351</v>
       </c>
       <c r="I48" t="s">
-        <v>337</v>
+        <v>352</v>
       </c>
       <c r="J48" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
+        <v>353</v>
+      </c>
+      <c r="K48" t="s"/>
+      <c r="L48" t="s"/>
+      <c r="M48" t="s"/>
+      <c r="N48" t="s"/>
+      <c r="O48" t="s"/>
+      <c r="P48" t="s"/>
+      <c r="Q48" t="s"/>
+      <c r="R48" t="s"/>
+      <c r="S48" t="s"/>
+      <c r="T48" t="s"/>
+      <c r="U48" t="s"/>
+      <c r="V48" t="s"/>
+      <c r="W48" t="s"/>
+      <c r="X48" t="s"/>
+      <c r="Y48" t="s"/>
+    </row>
+    <row r="49" spans="1:25">
       <c r="A49" s="1" t="n">
-        <v>5047</v>
+        <v>47</v>
       </c>
       <c r="B49" t="n">
         <v>41223</v>
       </c>
       <c r="C49" t="s">
-        <v>339</v>
+        <v>354</v>
       </c>
       <c r="D49" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E49" t="s">
-        <v>340</v>
+        <v>355</v>
       </c>
       <c r="F49" t="s">
-        <v>341</v>
+        <v>356</v>
       </c>
       <c r="G49" t="s">
-        <v>342</v>
+        <v>357</v>
       </c>
       <c r="H49" t="s">
-        <v>343</v>
+        <v>358</v>
       </c>
       <c r="I49" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="J49" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
+        <v>360</v>
+      </c>
+      <c r="K49" t="s"/>
+      <c r="L49" t="s"/>
+      <c r="M49" t="s"/>
+      <c r="N49" t="s"/>
+      <c r="O49" t="s">
+        <v>13</v>
+      </c>
+      <c r="P49" t="s"/>
+      <c r="Q49" t="s"/>
+      <c r="R49" t="s"/>
+      <c r="S49" t="s"/>
+      <c r="T49" t="s"/>
+      <c r="U49" t="s"/>
+      <c r="V49" t="s"/>
+      <c r="W49" t="s"/>
+      <c r="X49" t="s"/>
+      <c r="Y49" t="s"/>
+    </row>
+    <row r="50" spans="1:25">
       <c r="A50" s="1" t="n">
-        <v>5048</v>
+        <v>48</v>
       </c>
       <c r="B50" t="n">
         <v>41225</v>
       </c>
       <c r="C50" t="s">
-        <v>339</v>
+        <v>354</v>
       </c>
       <c r="D50" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E50" t="s">
-        <v>346</v>
+        <v>361</v>
       </c>
       <c r="F50" t="s">
-        <v>347</v>
+        <v>362</v>
       </c>
       <c r="G50" t="s">
-        <v>348</v>
+        <v>363</v>
       </c>
       <c r="H50" t="s">
-        <v>349</v>
+        <v>364</v>
       </c>
       <c r="I50" t="s">
-        <v>350</v>
+        <v>365</v>
       </c>
       <c r="J50" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
+        <v>366</v>
+      </c>
+      <c r="K50" t="s"/>
+      <c r="L50" t="s"/>
+      <c r="M50" t="s"/>
+      <c r="N50" t="s"/>
+      <c r="O50" t="s">
+        <v>13</v>
+      </c>
+      <c r="P50" t="s"/>
+      <c r="Q50" t="s"/>
+      <c r="R50" t="s"/>
+      <c r="S50" t="s"/>
+      <c r="T50" t="s"/>
+      <c r="U50" t="s"/>
+      <c r="V50" t="s"/>
+      <c r="W50" t="s"/>
+      <c r="X50" t="s"/>
+      <c r="Y50" t="s"/>
+    </row>
+    <row r="51" spans="1:25">
       <c r="A51" s="1" t="n">
-        <v>5399</v>
+        <v>49</v>
       </c>
       <c r="B51" t="n">
         <v>42268</v>
       </c>
       <c r="C51" t="s">
-        <v>352</v>
+        <v>367</v>
       </c>
       <c r="D51" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E51" t="s">
-        <v>353</v>
+        <v>368</v>
       </c>
       <c r="F51" t="s">
-        <v>354</v>
+        <v>369</v>
       </c>
       <c r="G51" t="s">
-        <v>355</v>
+        <v>370</v>
       </c>
       <c r="H51" t="s">
-        <v>356</v>
+        <v>371</v>
       </c>
       <c r="I51" t="s">
-        <v>357</v>
+        <v>372</v>
       </c>
       <c r="J51" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
+        <v>373</v>
+      </c>
+      <c r="K51" t="s"/>
+      <c r="L51" t="s"/>
+      <c r="M51" t="s"/>
+      <c r="N51" t="s"/>
+      <c r="O51" t="s">
+        <v>13</v>
+      </c>
+      <c r="P51" t="s"/>
+      <c r="Q51" t="s"/>
+      <c r="R51" t="s"/>
+      <c r="S51" t="s"/>
+      <c r="T51" t="s"/>
+      <c r="U51" t="s"/>
+      <c r="V51" t="s"/>
+      <c r="W51" t="s"/>
+      <c r="X51" t="s"/>
+      <c r="Y51" t="s"/>
+    </row>
+    <row r="52" spans="1:25">
       <c r="A52" s="1" t="n">
-        <v>5402</v>
+        <v>50</v>
       </c>
       <c r="B52" t="n">
         <v>42271</v>
       </c>
       <c r="C52" t="s">
-        <v>352</v>
+        <v>367</v>
       </c>
       <c r="D52" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E52" t="s">
-        <v>359</v>
+        <v>374</v>
       </c>
       <c r="F52" t="s">
-        <v>360</v>
+        <v>375</v>
       </c>
       <c r="G52" t="s">
-        <v>361</v>
+        <v>376</v>
       </c>
       <c r="H52" t="s">
-        <v>362</v>
+        <v>377</v>
       </c>
       <c r="I52" t="s">
-        <v>363</v>
+        <v>378</v>
       </c>
       <c r="J52" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
+        <v>379</v>
+      </c>
+      <c r="K52" t="s"/>
+      <c r="L52" t="s"/>
+      <c r="M52" t="s"/>
+      <c r="N52" t="s"/>
+      <c r="O52" t="s">
+        <v>13</v>
+      </c>
+      <c r="P52" t="s"/>
+      <c r="Q52" t="s"/>
+      <c r="R52" t="s"/>
+      <c r="S52" t="s"/>
+      <c r="T52" t="s"/>
+      <c r="U52" t="s"/>
+      <c r="V52" t="s"/>
+      <c r="W52" t="s"/>
+      <c r="X52" t="s"/>
+      <c r="Y52" t="s"/>
+    </row>
+    <row r="53" spans="1:25">
       <c r="A53" s="1" t="n">
-        <v>5413</v>
+        <v>51</v>
       </c>
       <c r="B53" t="n">
         <v>42283</v>
       </c>
       <c r="C53" t="s">
-        <v>365</v>
+        <v>380</v>
       </c>
       <c r="D53" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E53" t="s">
-        <v>366</v>
+        <v>381</v>
       </c>
       <c r="F53" t="s">
-        <v>367</v>
+        <v>382</v>
       </c>
       <c r="G53" t="s">
-        <v>368</v>
+        <v>383</v>
       </c>
       <c r="H53" t="s">
-        <v>369</v>
+        <v>384</v>
       </c>
       <c r="I53" t="s">
-        <v>370</v>
+        <v>385</v>
       </c>
       <c r="J53" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
+        <v>386</v>
+      </c>
+      <c r="K53" t="s"/>
+      <c r="L53" t="s"/>
+      <c r="M53" t="s"/>
+      <c r="N53" t="s"/>
+      <c r="O53" t="s">
+        <v>13</v>
+      </c>
+      <c r="P53" t="s"/>
+      <c r="Q53" t="s"/>
+      <c r="R53" t="s"/>
+      <c r="S53" t="s"/>
+      <c r="T53" t="s"/>
+      <c r="U53" t="s"/>
+      <c r="V53" t="s"/>
+      <c r="W53" t="s"/>
+      <c r="X53" t="s"/>
+      <c r="Y53" t="s"/>
+    </row>
+    <row r="54" spans="1:25">
       <c r="A54" s="1" t="n">
-        <v>5431</v>
+        <v>52</v>
       </c>
       <c r="B54" t="n">
         <v>42302</v>
       </c>
       <c r="C54" t="s">
-        <v>372</v>
+        <v>387</v>
       </c>
       <c r="D54" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="E54" t="s">
-        <v>373</v>
+        <v>388</v>
       </c>
       <c r="F54" t="s">
-        <v>374</v>
+        <v>389</v>
       </c>
       <c r="G54" t="s">
-        <v>375</v>
+        <v>390</v>
       </c>
       <c r="H54" t="s">
-        <v>376</v>
+        <v>391</v>
       </c>
       <c r="I54" t="s">
-        <v>377</v>
+        <v>392</v>
       </c>
       <c r="J54" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
+        <v>393</v>
+      </c>
+      <c r="K54" t="s"/>
+      <c r="L54" t="s"/>
+      <c r="M54" t="s"/>
+      <c r="N54" t="s"/>
+      <c r="O54" t="s">
+        <v>13</v>
+      </c>
+      <c r="P54" t="s"/>
+      <c r="Q54" t="s"/>
+      <c r="R54" t="s"/>
+      <c r="S54" t="s"/>
+      <c r="T54" t="s"/>
+      <c r="U54" t="s"/>
+      <c r="V54" t="s"/>
+      <c r="W54" t="s"/>
+      <c r="X54" t="s"/>
+      <c r="Y54" t="s"/>
+    </row>
+    <row r="55" spans="1:25">
       <c r="A55" s="1" t="n">
-        <v>5462</v>
+        <v>53</v>
       </c>
       <c r="B55" t="n">
         <v>42349</v>
       </c>
       <c r="C55" t="s">
-        <v>379</v>
+        <v>394</v>
       </c>
       <c r="D55" t="s">
-        <v>380</v>
+        <v>395</v>
       </c>
       <c r="E55" t="s">
-        <v>381</v>
+        <v>396</v>
       </c>
       <c r="F55" t="s">
-        <v>382</v>
+        <v>397</v>
       </c>
       <c r="G55" t="s">
-        <v>383</v>
+        <v>398</v>
       </c>
       <c r="H55" t="s">
-        <v>384</v>
+        <v>399</v>
       </c>
       <c r="I55" t="s">
-        <v>385</v>
+        <v>400</v>
       </c>
       <c r="J55" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
+        <v>401</v>
+      </c>
+      <c r="K55" t="s"/>
+      <c r="L55" t="s"/>
+      <c r="M55" t="s"/>
+      <c r="N55" t="s"/>
+      <c r="O55" t="s"/>
+      <c r="P55" t="s"/>
+      <c r="Q55" t="s"/>
+      <c r="R55" t="s"/>
+      <c r="S55" t="s"/>
+      <c r="T55" t="s"/>
+      <c r="U55" t="s"/>
+      <c r="V55" t="s"/>
+      <c r="W55" t="s"/>
+      <c r="X55" t="s"/>
+      <c r="Y55" t="s"/>
+    </row>
+    <row r="56" spans="1:25">
       <c r="A56" s="1" t="n">
-        <v>5524</v>
+        <v>54</v>
       </c>
       <c r="B56" t="n">
         <v>42450</v>
       </c>
       <c r="C56" t="s">
-        <v>387</v>
+        <v>402</v>
       </c>
       <c r="D56" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E56" t="s">
-        <v>388</v>
+        <v>403</v>
       </c>
       <c r="F56" t="s">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="G56" t="s">
-        <v>390</v>
+        <v>405</v>
       </c>
       <c r="H56" t="s">
-        <v>391</v>
+        <v>406</v>
       </c>
       <c r="I56" t="s">
-        <v>392</v>
+        <v>407</v>
       </c>
       <c r="J56" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
+        <v>408</v>
+      </c>
+      <c r="K56" t="s"/>
+      <c r="L56" t="s"/>
+      <c r="M56" t="s"/>
+      <c r="N56" t="s"/>
+      <c r="O56" t="s"/>
+      <c r="P56" t="s"/>
+      <c r="Q56" t="s"/>
+      <c r="R56" t="s"/>
+      <c r="S56" t="s"/>
+      <c r="T56" t="s"/>
+      <c r="U56" t="s"/>
+      <c r="V56" t="s"/>
+      <c r="W56" t="s"/>
+      <c r="X56" t="s"/>
+      <c r="Y56" t="s"/>
+    </row>
+    <row r="57" spans="1:25">
       <c r="A57" s="1" t="n">
-        <v>5526</v>
+        <v>55</v>
       </c>
       <c r="B57" t="n">
         <v>42452</v>
       </c>
       <c r="C57" t="s">
-        <v>394</v>
+        <v>409</v>
       </c>
       <c r="D57" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E57" t="s">
-        <v>395</v>
+        <v>410</v>
       </c>
       <c r="F57" t="s">
-        <v>396</v>
+        <v>411</v>
       </c>
       <c r="G57" t="s">
-        <v>397</v>
+        <v>412</v>
       </c>
       <c r="H57" t="s">
-        <v>398</v>
+        <v>413</v>
       </c>
       <c r="I57" t="s">
-        <v>399</v>
+        <v>414</v>
       </c>
       <c r="J57" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
+        <v>415</v>
+      </c>
+      <c r="K57" t="s"/>
+      <c r="L57" t="s"/>
+      <c r="M57" t="s"/>
+      <c r="N57" t="s"/>
+      <c r="O57" t="s"/>
+      <c r="P57" t="s"/>
+      <c r="Q57" t="s"/>
+      <c r="R57" t="s"/>
+      <c r="S57" t="s"/>
+      <c r="T57" t="s"/>
+      <c r="U57" t="s"/>
+      <c r="V57" t="s"/>
+      <c r="W57" t="s"/>
+      <c r="X57" t="s"/>
+      <c r="Y57" t="s"/>
+    </row>
+    <row r="58" spans="1:25">
       <c r="A58" s="1" t="n">
-        <v>5666</v>
+        <v>56</v>
       </c>
       <c r="B58" t="n">
         <v>43000</v>
       </c>
       <c r="C58" t="s">
-        <v>401</v>
+        <v>416</v>
       </c>
       <c r="D58" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E58" t="s">
-        <v>402</v>
+        <v>417</v>
       </c>
       <c r="F58" t="s">
-        <v>403</v>
+        <v>418</v>
       </c>
       <c r="G58" t="s">
-        <v>404</v>
+        <v>419</v>
       </c>
       <c r="H58" t="s">
-        <v>405</v>
+        <v>420</v>
       </c>
       <c r="I58" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
       <c r="J58" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
+        <v>422</v>
+      </c>
+      <c r="K58" t="s"/>
+      <c r="L58" t="s"/>
+      <c r="M58" t="s"/>
+      <c r="N58" t="s"/>
+      <c r="O58" t="s"/>
+      <c r="P58" t="s"/>
+      <c r="Q58" t="s"/>
+      <c r="R58" t="s"/>
+      <c r="S58" t="s"/>
+      <c r="T58" t="s"/>
+      <c r="U58" t="s"/>
+      <c r="V58" t="s"/>
+      <c r="W58" t="s"/>
+      <c r="X58" t="s"/>
+      <c r="Y58" t="s"/>
+    </row>
+    <row r="59" spans="1:25">
       <c r="A59" s="1" t="n">
-        <v>5869</v>
+        <v>57</v>
       </c>
       <c r="B59" t="n">
         <v>43393</v>
       </c>
       <c r="C59" t="s"/>
       <c r="D59" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E59" t="s">
-        <v>408</v>
+        <v>423</v>
       </c>
       <c r="F59" t="s">
-        <v>409</v>
+        <v>424</v>
       </c>
       <c r="G59" t="s">
-        <v>410</v>
+        <v>425</v>
       </c>
       <c r="H59" t="s">
-        <v>411</v>
+        <v>426</v>
       </c>
       <c r="I59" t="s">
-        <v>412</v>
+        <v>427</v>
       </c>
       <c r="J59" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
+        <v>428</v>
+      </c>
+      <c r="K59" t="s"/>
+      <c r="L59" t="s"/>
+      <c r="M59" t="s"/>
+      <c r="N59" t="s"/>
+      <c r="O59" t="s">
+        <v>13</v>
+      </c>
+      <c r="P59" t="s"/>
+      <c r="Q59" t="s"/>
+      <c r="R59" t="s"/>
+      <c r="S59" t="s"/>
+      <c r="T59" t="s"/>
+      <c r="U59" t="s"/>
+      <c r="V59" t="s"/>
+      <c r="W59" t="s"/>
+      <c r="X59" t="s"/>
+      <c r="Y59" t="s"/>
+    </row>
+    <row r="60" spans="1:25">
       <c r="A60" s="1" t="n">
-        <v>6118</v>
+        <v>58</v>
       </c>
       <c r="B60" t="n">
         <v>43759</v>
       </c>
       <c r="C60" t="s">
-        <v>414</v>
+        <v>429</v>
       </c>
       <c r="D60" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E60" t="s">
-        <v>415</v>
+        <v>430</v>
       </c>
       <c r="F60" t="s">
-        <v>416</v>
+        <v>431</v>
       </c>
       <c r="G60" t="s">
-        <v>417</v>
+        <v>432</v>
       </c>
       <c r="H60" t="s">
-        <v>418</v>
+        <v>433</v>
       </c>
       <c r="I60" t="s">
-        <v>419</v>
+        <v>434</v>
       </c>
       <c r="J60" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
+        <v>435</v>
+      </c>
+      <c r="K60" t="s"/>
+      <c r="L60" t="s"/>
+      <c r="M60" t="s"/>
+      <c r="N60" t="s"/>
+      <c r="O60" t="s"/>
+      <c r="P60" t="s"/>
+      <c r="Q60" t="s"/>
+      <c r="R60" t="s"/>
+      <c r="S60" t="s"/>
+      <c r="T60" t="s"/>
+      <c r="U60" t="s"/>
+      <c r="V60" t="s"/>
+      <c r="W60" t="s"/>
+      <c r="X60" t="s"/>
+      <c r="Y60" t="s"/>
+    </row>
+    <row r="61" spans="1:25">
       <c r="A61" s="1" t="n">
-        <v>6142</v>
+        <v>59</v>
       </c>
       <c r="B61" t="n">
         <v>43784</v>
       </c>
       <c r="C61" t="s">
-        <v>414</v>
+        <v>429</v>
       </c>
       <c r="D61" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E61" t="s">
-        <v>421</v>
+        <v>436</v>
       </c>
       <c r="F61" t="s">
-        <v>422</v>
+        <v>437</v>
       </c>
       <c r="G61" t="s">
-        <v>423</v>
+        <v>438</v>
       </c>
       <c r="H61" t="s">
-        <v>424</v>
+        <v>439</v>
       </c>
       <c r="I61" t="s">
-        <v>425</v>
+        <v>440</v>
       </c>
       <c r="J61" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
+        <v>441</v>
+      </c>
+      <c r="K61" t="s"/>
+      <c r="L61" t="s"/>
+      <c r="M61" t="s"/>
+      <c r="N61" t="s"/>
+      <c r="O61" t="s"/>
+      <c r="P61" t="s"/>
+      <c r="Q61" t="s"/>
+      <c r="R61" t="s"/>
+      <c r="S61" t="s"/>
+      <c r="T61" t="s"/>
+      <c r="U61" t="s"/>
+      <c r="V61" t="s"/>
+      <c r="W61" t="s"/>
+      <c r="X61" t="s"/>
+      <c r="Y61" t="s"/>
+    </row>
+    <row r="62" spans="1:25">
       <c r="A62" s="1" t="n">
-        <v>6457</v>
+        <v>60</v>
       </c>
       <c r="B62" t="n">
         <v>44358</v>
       </c>
       <c r="C62" t="s">
-        <v>427</v>
+        <v>442</v>
       </c>
       <c r="D62" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E62" t="s">
-        <v>428</v>
+        <v>443</v>
       </c>
       <c r="F62" t="s">
-        <v>429</v>
+        <v>444</v>
       </c>
       <c r="G62" t="s">
-        <v>430</v>
+        <v>445</v>
       </c>
       <c r="H62" t="s">
-        <v>431</v>
+        <v>446</v>
       </c>
       <c r="I62" t="s">
-        <v>432</v>
+        <v>447</v>
       </c>
       <c r="J62" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
+        <v>448</v>
+      </c>
+      <c r="K62" t="s"/>
+      <c r="L62" t="s"/>
+      <c r="M62" t="s"/>
+      <c r="N62" t="s"/>
+      <c r="O62" t="s">
+        <v>13</v>
+      </c>
+      <c r="P62" t="s"/>
+      <c r="Q62" t="s"/>
+      <c r="R62" t="s"/>
+      <c r="S62" t="s"/>
+      <c r="T62" t="s"/>
+      <c r="U62" t="s"/>
+      <c r="V62" t="s"/>
+      <c r="W62" t="s"/>
+      <c r="X62" t="s"/>
+      <c r="Y62" t="s"/>
+    </row>
+    <row r="63" spans="1:25">
       <c r="A63" s="1" t="n">
-        <v>6582</v>
+        <v>61</v>
       </c>
       <c r="B63" t="n">
         <v>44550</v>
       </c>
       <c r="C63" t="s">
-        <v>434</v>
+        <v>449</v>
       </c>
       <c r="D63" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E63" t="s">
-        <v>435</v>
+        <v>450</v>
       </c>
       <c r="F63" t="s">
-        <v>436</v>
+        <v>451</v>
       </c>
       <c r="G63" t="s">
-        <v>437</v>
+        <v>452</v>
       </c>
       <c r="H63" t="s">
-        <v>438</v>
+        <v>453</v>
       </c>
       <c r="I63" t="s">
-        <v>439</v>
+        <v>454</v>
       </c>
       <c r="J63" t="s">
-        <v>440</v>
-      </c>
+        <v>455</v>
+      </c>
+      <c r="K63" t="s"/>
+      <c r="L63" t="s"/>
+      <c r="M63" t="s"/>
+      <c r="N63" t="s"/>
+      <c r="O63" t="s"/>
+      <c r="P63" t="s"/>
+      <c r="Q63" t="s"/>
+      <c r="R63" t="s"/>
+      <c r="S63" t="s"/>
+      <c r="T63" t="s"/>
+      <c r="U63" t="s"/>
+      <c r="V63" t="s"/>
+      <c r="W63" t="s"/>
+      <c r="X63" t="s"/>
+      <c r="Y63" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>